<commit_message>
se arregló item que daba error con el Span en Hogar
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E795EBDA-16F6-46AF-8D65-A51F3AD41A28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400491DB-78FA-47D8-8124-E1C7A4D7BFFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,9 +65,6 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>SmokeSiete</t>
-  </si>
-  <si>
     <t>PRC015</t>
   </si>
   <si>
@@ -75,6 +72,9 @@
   </si>
   <si>
     <t>ZAZ123SPRC015</t>
+  </si>
+  <si>
+    <t>SmokeOcho</t>
   </si>
 </sst>
 </file>
@@ -410,7 +410,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,16 +436,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C2">
-        <v>21546996</v>
+        <v>21546999</v>
       </c>
       <c r="D2">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -506,13 +506,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se habilitó Centro de Confianza en Excel para Datasources y se agrego tesCase de Anuliaciones
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400491DB-78FA-47D8-8124-E1C7A4D7BFFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41120CDC-603F-4CA1-827D-F167674F1DF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
     <t>ZAZ123SPRC015</t>
   </si>
   <si>
-    <t>SmokeOcho</t>
+    <t>SmokeDiez</t>
   </si>
 </sst>
 </file>
@@ -410,7 +410,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,10 +442,10 @@
         <v>12</v>
       </c>
       <c r="C2">
-        <v>21546999</v>
+        <v>21546910</v>
       </c>
       <c r="D2">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se modif datos para smoke en preprod despligue R31
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41120CDC-603F-4CA1-827D-F167674F1DF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B114BCA-1EC5-41D7-947D-E2F1F8A7C60C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DatosCuenta" sheetId="1" r:id="rId1"/>
@@ -65,16 +65,16 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>PRC015</t>
-  </si>
-  <si>
-    <t>ABC12SPRC015</t>
-  </si>
-  <si>
-    <t>ZAZ123SPRC015</t>
-  </si>
-  <si>
-    <t>SmokeDiez</t>
+    <t>SmokeOnce</t>
+  </si>
+  <si>
+    <t>PRC016</t>
+  </si>
+  <si>
+    <t>ABC12SPRC016</t>
+  </si>
+  <si>
+    <t>ZAZ123SPRC016</t>
   </si>
 </sst>
 </file>
@@ -409,8 +409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,16 +436,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>21546910</v>
       </c>
       <c r="D2">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -459,7 +459,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,7 +471,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>610</v>
+        <v>611</v>
       </c>
     </row>
   </sheetData>
@@ -484,7 +484,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,13 +506,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -525,7 +525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2DEA8B-0CD5-444B-B1FB-D4111E0F6DDF}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -538,7 +538,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>21840815</v>
+        <v>21840816</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se sube para ejecutar en preprod
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B114BCA-1EC5-41D7-947D-E2F1F8A7C60C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E38657-458C-4D19-BFFE-4174340A1FC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DatosCuenta" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
@@ -65,16 +65,19 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>SmokeOnce</t>
-  </si>
-  <si>
-    <t>PRC016</t>
-  </si>
-  <si>
-    <t>ABC12SPRC016</t>
-  </si>
-  <si>
-    <t>ZAZ123SPRC016</t>
+    <t>PRC017</t>
+  </si>
+  <si>
+    <t>ABC12SPRC017</t>
+  </si>
+  <si>
+    <t>ZAZ123SPRC017</t>
+  </si>
+  <si>
+    <t>SmokeDoceName</t>
+  </si>
+  <si>
+    <t>SmokeDoceLastName</t>
   </si>
 </sst>
 </file>
@@ -409,8 +412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,16 +439,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C2">
-        <v>21546910</v>
+        <v>21546911</v>
       </c>
       <c r="D2">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -459,7 +462,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,7 +474,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>611</v>
+        <v>612</v>
       </c>
     </row>
   </sheetData>
@@ -484,7 +487,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,13 +509,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -525,7 +528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2DEA8B-0CD5-444B-B1FB-D4111E0F6DDF}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -538,7 +541,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>21840816</v>
+        <v>21840817</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se sube nueva version con Rehabilitar
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E38657-458C-4D19-BFFE-4174340A1FC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36445FDC-1DBE-4CA4-8B7D-B9FAF8795B1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DatosCuenta" sheetId="1" r:id="rId1"/>
@@ -65,19 +65,19 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>PRC017</t>
-  </si>
-  <si>
-    <t>ABC12SPRC017</t>
-  </si>
-  <si>
-    <t>ZAZ123SPRC017</t>
-  </si>
-  <si>
-    <t>SmokeDoceName</t>
-  </si>
-  <si>
-    <t>SmokeDoceLastName</t>
+    <t>SmokeLastName</t>
+  </si>
+  <si>
+    <t>SmokeName</t>
+  </si>
+  <si>
+    <t>SMA001</t>
+  </si>
+  <si>
+    <t>ABC12SSMA001</t>
+  </si>
+  <si>
+    <t>ZAZ123SSMA001</t>
   </si>
 </sst>
 </file>
@@ -412,8 +412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,16 +439,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C2">
-        <v>21546911</v>
+        <v>20111100</v>
       </c>
       <c r="D2">
-        <v>144</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -474,7 +474,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>612</v>
+        <v>620</v>
       </c>
     </row>
   </sheetData>
@@ -487,7 +487,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,13 +509,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -528,7 +528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2DEA8B-0CD5-444B-B1FB-D4111E0F6DDF}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -541,7 +541,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>21840817</v>
+        <v>21200100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se sube cambios de data para smoke catroce en QA
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36445FDC-1DBE-4CA4-8B7D-B9FAF8795B1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C263A668-C946-4419-9366-298F25CC63A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,19 +65,19 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>SmokeLastName</t>
-  </si>
-  <si>
-    <t>SmokeName</t>
-  </si>
-  <si>
-    <t>SMA001</t>
-  </si>
-  <si>
-    <t>ABC12SSMA001</t>
-  </si>
-  <si>
-    <t>ZAZ123SSMA001</t>
+    <t>SmokeCatorce</t>
+  </si>
+  <si>
+    <t>SmokeLastNCatorce</t>
+  </si>
+  <si>
+    <t>SMA002</t>
+  </si>
+  <si>
+    <t>ABC12SSMA002</t>
+  </si>
+  <si>
+    <t>ZAZ123SSMA002</t>
   </si>
 </sst>
 </file>
@@ -439,16 +439,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
       <c r="C2">
-        <v>20111100</v>
+        <v>20111101</v>
       </c>
       <c r="D2">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -474,7 +474,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>620</v>
+        <v>621</v>
       </c>
     </row>
   </sheetData>
@@ -487,7 +487,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +541,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>21200100</v>
+        <v>21200101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se modif datos de cuenta
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4702FDDA-94CF-49EC-A8B4-BEB7261A3D47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD4CED9-F59A-495E-882E-E6D3EEE35541}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DatosCuenta" sheetId="1" r:id="rId1"/>
@@ -65,19 +65,19 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>SMA002</t>
-  </si>
-  <si>
-    <t>ABC12SSMA002</t>
-  </si>
-  <si>
-    <t>ZAZ123SSMA002</t>
-  </si>
-  <si>
-    <t>SmokeUno</t>
-  </si>
-  <si>
-    <t>SmokeLastNUno</t>
+    <t>SmokeDos</t>
+  </si>
+  <si>
+    <t>SmokeLastDos</t>
+  </si>
+  <si>
+    <t>SMA003</t>
+  </si>
+  <si>
+    <t>ABC12SSMA003</t>
+  </si>
+  <si>
+    <t>ZAZ123SSMA003</t>
   </si>
 </sst>
 </file>
@@ -412,8 +412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,16 +439,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>20111101</v>
+        <v>20111102</v>
       </c>
       <c r="D2">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -462,7 +462,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,7 +474,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
   </sheetData>
@@ -486,7 +486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B4D3337-C598-431D-875D-6881D8F6F2F1}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
@@ -509,13 +509,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -529,7 +529,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +541,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>21200101</v>
+        <v>21200102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se nuevo la cuenta falló en SISE
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD4CED9-F59A-495E-882E-E6D3EEE35541}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A56356-ED05-4D8C-B577-C5B6FC0406E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,19 +65,19 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>SmokeDos</t>
-  </si>
-  <si>
-    <t>SmokeLastDos</t>
-  </si>
-  <si>
-    <t>SMA003</t>
-  </si>
-  <si>
-    <t>ABC12SSMA003</t>
-  </si>
-  <si>
-    <t>ZAZ123SSMA003</t>
+    <t>SmokeM</t>
+  </si>
+  <si>
+    <t>SmokeLastM</t>
+  </si>
+  <si>
+    <t>SMA004</t>
+  </si>
+  <si>
+    <t>ABC12SSMA004</t>
+  </si>
+  <si>
+    <t>ZAZ123SSMA004</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,10 +445,10 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <v>20111102</v>
+        <v>20100100</v>
       </c>
       <c r="D2">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -474,7 +474,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>622</v>
+        <v>623</v>
       </c>
     </row>
   </sheetData>
@@ -529,7 +529,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +541,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>21200102</v>
+        <v>21200103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se nuevo dio error la cuenta en SISE
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A56356-ED05-4D8C-B577-C5B6FC0406E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC546DA6-A4C9-4AD7-9545-7A779D977A5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DatosCuenta" sheetId="1" r:id="rId1"/>
@@ -65,19 +65,19 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>SmokeM</t>
-  </si>
-  <si>
-    <t>SmokeLastM</t>
-  </si>
-  <si>
-    <t>SMA004</t>
-  </si>
-  <si>
-    <t>ABC12SSMA004</t>
-  </si>
-  <si>
-    <t>ZAZ123SSMA004</t>
+    <t>SmokeMP</t>
+  </si>
+  <si>
+    <t>SmokeLastMP</t>
+  </si>
+  <si>
+    <t>SMA005</t>
+  </si>
+  <si>
+    <t>ABC12SSMA005</t>
+  </si>
+  <si>
+    <t>ZAZ123SSMA005</t>
   </si>
 </sst>
 </file>
@@ -412,7 +412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -445,10 +445,10 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <v>20100100</v>
+        <v>20100101</v>
       </c>
       <c r="D2">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -474,7 +474,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>623</v>
+        <v>624</v>
       </c>
     </row>
   </sheetData>
@@ -528,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2DEA8B-0CD5-444B-B1FB-D4111E0F6DDF}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +541,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>21200103</v>
+        <v>21200104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se agrega cuenta con datos de pablo
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC546DA6-A4C9-4AD7-9545-7A779D977A5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F18A0C-F320-403A-B699-43ABB4750A29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,19 +65,19 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>SmokeMP</t>
-  </si>
-  <si>
-    <t>SmokeLastMP</t>
-  </si>
-  <si>
-    <t>SMA005</t>
-  </si>
-  <si>
-    <t>ABC12SSMA005</t>
-  </si>
-  <si>
-    <t>ZAZ123SSMA005</t>
+    <t>Burri</t>
+  </si>
+  <si>
+    <t>Pablo Martin</t>
+  </si>
+  <si>
+    <t>SMA006</t>
+  </si>
+  <si>
+    <t>ABC12SSMA006</t>
+  </si>
+  <si>
+    <t>ZAZ123SSMA006</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,7 +445,7 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <v>20100101</v>
+        <v>28263674</v>
       </c>
       <c r="D2">
         <v>104</v>
@@ -474,7 +474,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>624</v>
+        <v>625</v>
       </c>
     </row>
   </sheetData>
@@ -529,7 +529,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +541,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>21200104</v>
+        <v>21200105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
su sube con tros datos de cuenta
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F18A0C-F320-403A-B699-43ABB4750A29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3818AC-9564-4372-A29F-087D9B4B61CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DatosCuenta" sheetId="1" r:id="rId1"/>
@@ -65,12 +65,6 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>Burri</t>
-  </si>
-  <si>
-    <t>Pablo Martin</t>
-  </si>
-  <si>
     <t>SMA006</t>
   </si>
   <si>
@@ -78,6 +72,12 @@
   </si>
   <si>
     <t>ZAZ123SSMA006</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lospennato</t>
+  </si>
+  <si>
+    <t>Andrea Mariela</t>
   </si>
 </sst>
 </file>
@@ -412,8 +412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,13 +439,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2">
-        <v>28263674</v>
+        <v>27088681</v>
       </c>
       <c r="D2">
         <v>104</v>
@@ -509,13 +509,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -528,7 +528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2DEA8B-0CD5-444B-B1FB-D4111E0F6DDF}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
se sube data para correr Smoke En PreProd después de la actualziación de Oracle de la máquinas virtuales
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4246195C-D241-48E0-A54E-28102B096EBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFF0819-3D7D-4EA9-821C-D5C83A0C1FF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DatosCuenta" sheetId="1" r:id="rId1"/>
@@ -65,12 +65,6 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>PruebaCuenta</t>
-  </si>
-  <si>
-    <t>Apellido</t>
-  </si>
-  <si>
     <t>SMA008</t>
   </si>
   <si>
@@ -78,6 +72,12 @@
   </si>
   <si>
     <t>ZAZ123SSMA008</t>
+  </si>
+  <si>
+    <t>PruebaSmoke</t>
+  </si>
+  <si>
+    <t>ApellidoSmoke</t>
   </si>
 </sst>
 </file>
@@ -412,8 +412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,16 +439,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2">
-        <v>27100101</v>
+        <v>27100102</v>
       </c>
       <c r="D2">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -509,13 +509,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -528,7 +528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2DEA8B-0CD5-444B-B1FB-D4111E0F6DDF}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
se modif data para smoke en preprod
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFF0819-3D7D-4EA9-821C-D5C83A0C1FF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4791D3E3-1B0E-420F-BEED-7D67D2057F1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,10 +74,10 @@
     <t>ZAZ123SSMA008</t>
   </si>
   <si>
-    <t>PruebaSmoke</t>
-  </si>
-  <si>
-    <t>ApellidoSmoke</t>
+    <t>PMSmoke</t>
+  </si>
+  <si>
+    <t>ApellidoPMSmoke</t>
   </si>
 </sst>
 </file>
@@ -445,10 +445,10 @@
         <v>13</v>
       </c>
       <c r="C2">
-        <v>27100102</v>
+        <v>27100105</v>
       </c>
       <c r="D2">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se prueba parametros en jenkins para SmokePagoReversa
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4791D3E3-1B0E-420F-BEED-7D67D2057F1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD12C2B9-295E-43E4-B70B-98625EEC7E9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DatosCuenta" sheetId="1" r:id="rId1"/>
@@ -65,19 +65,19 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>SMA008</t>
-  </si>
-  <si>
-    <t>ABC12SSMA008</t>
-  </si>
-  <si>
-    <t>ZAZ123SSMA008</t>
-  </si>
-  <si>
-    <t>PMSmoke</t>
-  </si>
-  <si>
-    <t>ApellidoPMSmoke</t>
+    <t>PMSmokeT</t>
+  </si>
+  <si>
+    <t>ApellidoPMSmokeT</t>
+  </si>
+  <si>
+    <t>SMA009</t>
+  </si>
+  <si>
+    <t>ABC12SSMA009</t>
+  </si>
+  <si>
+    <t>ZAZ123SSMA009</t>
   </si>
 </sst>
 </file>
@@ -412,8 +412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,13 +439,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>27100105</v>
+        <v>27100106</v>
       </c>
       <c r="D2">
         <v>108</v>
@@ -474,7 +474,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
   </sheetData>
@@ -509,13 +509,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -528,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2DEA8B-0CD5-444B-B1FB-D4111E0F6DDF}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +541,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>21200107</v>
+        <v>21200108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modificación de Data para Smoke QA Mayo R33
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD12C2B9-295E-43E4-B70B-98625EEC7E9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9019D377-E9BC-4FDA-84FD-66094463F39A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,19 +65,19 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>PMSmokeT</t>
-  </si>
-  <si>
-    <t>ApellidoPMSmokeT</t>
-  </si>
-  <si>
-    <t>SMA009</t>
-  </si>
-  <si>
-    <t>ABC12SSMA009</t>
-  </si>
-  <si>
-    <t>ZAZ123SSMA009</t>
+    <t>SmokeMayo</t>
+  </si>
+  <si>
+    <t>SmokeMayoLastName</t>
+  </si>
+  <si>
+    <t>SMA010</t>
+  </si>
+  <si>
+    <t>ABC12SSMA010</t>
+  </si>
+  <si>
+    <t>ZAZ123SSMA010</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,10 +445,10 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <v>27100106</v>
+        <v>27100107</v>
       </c>
       <c r="D2">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -474,7 +474,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>628</v>
+        <v>629</v>
       </c>
     </row>
   </sheetData>
@@ -529,7 +529,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +541,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>21200108</v>
+        <v>21200109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se modificada data para smoke en pre prod
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9019D377-E9BC-4FDA-84FD-66094463F39A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B6B679-F213-4876-AE49-B1A693446C16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,12 +65,6 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>SmokeMayo</t>
-  </si>
-  <si>
-    <t>SmokeMayoLastName</t>
-  </si>
-  <si>
     <t>SMA010</t>
   </si>
   <si>
@@ -78,6 +72,12 @@
   </si>
   <si>
     <t>ZAZ123SSMA010</t>
+  </si>
+  <si>
+    <t>SmokePre</t>
+  </si>
+  <si>
+    <t>SmokePreHotFix</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,10 +439,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>27100107</v>
@@ -509,13 +509,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se midifica data para prueba con Pablo del HotFix - mensajerias
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B6B679-F213-4876-AE49-B1A693446C16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7656F973-4359-44CA-B988-04DC7A443909}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,19 +65,19 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>SMA010</t>
-  </si>
-  <si>
-    <t>ABC12SSMA010</t>
-  </si>
-  <si>
-    <t>ZAZ123SSMA010</t>
-  </si>
-  <si>
-    <t>SmokePre</t>
-  </si>
-  <si>
-    <t>SmokePreHotFix</t>
+    <t>SmokePreHotFixDOs</t>
+  </si>
+  <si>
+    <t>SmokePreDOS</t>
+  </si>
+  <si>
+    <t>SMA011</t>
+  </si>
+  <si>
+    <t>ABC12SSMA011</t>
+  </si>
+  <si>
+    <t>ZAZ123SSMA011</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,16 +439,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C2">
-        <v>27100107</v>
+        <v>27100108</v>
       </c>
       <c r="D2">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -462,7 +462,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,7 +474,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>629</v>
+        <v>630</v>
       </c>
     </row>
   </sheetData>
@@ -509,13 +509,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -529,7 +529,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +541,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>21200109</v>
+        <v>21200110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se modifica datos para smoke preprod
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5D1BBB-9928-449D-9636-F8D560541FDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22344DC3-69B0-4F22-8EC2-920DF888C71D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,13 +71,13 @@
     <t>SmokePreNameTRES</t>
   </si>
   <si>
-    <t>SMA012</t>
-  </si>
-  <si>
-    <t>ABC12SSMA012</t>
-  </si>
-  <si>
-    <t>ZAZ123SSMA012</t>
+    <t>SMA013</t>
+  </si>
+  <si>
+    <t>ABC12SSMA013</t>
+  </si>
+  <si>
+    <t>ZAZ123SSMA013</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,10 +445,10 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <v>27100108</v>
+        <v>27100110</v>
       </c>
       <c r="D2">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -474,7 +474,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>631</v>
+        <v>632</v>
       </c>
     </row>
   </sheetData>
@@ -487,7 +487,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C4"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,7 +529,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +541,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>21200111</v>
+        <v>21200112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se modifica data oara smoke en prepros tercera vez
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22344DC3-69B0-4F22-8EC2-920DF888C71D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7223534-7EA0-422C-99FE-DF0CEF0083BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DatosCuenta" sheetId="1" r:id="rId1"/>
@@ -65,19 +65,19 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>SmokePreTRES</t>
-  </si>
-  <si>
-    <t>SmokePreNameTRES</t>
-  </si>
-  <si>
-    <t>SMA013</t>
-  </si>
-  <si>
-    <t>ABC12SSMA013</t>
-  </si>
-  <si>
-    <t>ZAZ123SSMA013</t>
+    <t>SmokePreCuatro</t>
+  </si>
+  <si>
+    <t>SmokePreNameCuatro</t>
+  </si>
+  <si>
+    <t>SMA014</t>
+  </si>
+  <si>
+    <t>ABC12SSMA014</t>
+  </si>
+  <si>
+    <t>ZAZ123SSMA014</t>
   </si>
 </sst>
 </file>
@@ -412,8 +412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,10 +445,10 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <v>27100110</v>
+        <v>27100111</v>
       </c>
       <c r="D2">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -474,7 +474,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>632</v>
+        <v>633</v>
       </c>
     </row>
   </sheetData>
@@ -528,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2DEA8B-0CD5-444B-B1FB-D4111E0F6DDF}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +541,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>21200112</v>
+        <v>21200113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se modificA data paea regresion cinco en pre prod
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7223534-7EA0-422C-99FE-DF0CEF0083BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC5C848-6683-4F76-88E7-9F95CCFF995F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,19 +65,19 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>SmokePreCuatro</t>
-  </si>
-  <si>
-    <t>SmokePreNameCuatro</t>
-  </si>
-  <si>
-    <t>SMA014</t>
-  </si>
-  <si>
-    <t>ABC12SSMA014</t>
-  </si>
-  <si>
-    <t>ZAZ123SSMA014</t>
+    <t>SmokePreCinco</t>
+  </si>
+  <si>
+    <t>SmokePreNameCinco</t>
+  </si>
+  <si>
+    <t>SMA015</t>
+  </si>
+  <si>
+    <t>ABC12SSMA015</t>
+  </si>
+  <si>
+    <t>ZAZ123SSMA015</t>
   </si>
 </sst>
 </file>
@@ -445,10 +445,10 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <v>27100111</v>
+        <v>27100112</v>
       </c>
       <c r="D2">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -474,7 +474,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
   </sheetData>
@@ -529,7 +529,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +541,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>21200113</v>
+        <v>21200114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se cambia data para smoke en qa
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F20492A-6007-46DC-A727-E799F8864B9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2395E5E8-44AB-49D6-B78A-79C685E513E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,19 +65,19 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>SMA016</t>
-  </si>
-  <si>
-    <t>ABC12SSMA016</t>
-  </si>
-  <si>
-    <t>ZAZ123SSMA016</t>
-  </si>
-  <si>
-    <t>SmokePreSeis</t>
-  </si>
-  <si>
-    <t>SmokePreNameSeis</t>
+    <t>SmokeQAUno</t>
+  </si>
+  <si>
+    <t>SmokeQANameUno</t>
+  </si>
+  <si>
+    <t>SMA017</t>
+  </si>
+  <si>
+    <t>ABC12SSMA017</t>
+  </si>
+  <si>
+    <t>ZAZ123SSMA017</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,16 +439,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>27100113</v>
+        <v>27100114</v>
       </c>
       <c r="D2">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -474,7 +474,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
   </sheetData>
@@ -509,13 +509,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -541,7 +541,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>21200115</v>
+        <v>21200117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se mejora parte de AP seleccion de metodo de pago No cuotas se mofifica data para smoke en preprod despues de trabajos de Oracle Se modifica testRun de Smoke
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2395E5E8-44AB-49D6-B78A-79C685E513E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141753F2-688C-483B-A0AE-80D4D22EF63E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,12 +65,6 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>SmokeQAUno</t>
-  </si>
-  <si>
-    <t>SmokeQANameUno</t>
-  </si>
-  <si>
     <t>SMA017</t>
   </si>
   <si>
@@ -78,6 +72,12 @@
   </si>
   <si>
     <t>ZAZ123SSMA017</t>
+  </si>
+  <si>
+    <t>SmokPreSiete</t>
+  </si>
+  <si>
+    <t>SmokePreProdNamSiete</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,10 +439,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>27100114</v>
@@ -487,7 +487,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,13 +509,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -529,7 +529,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
se modif data para Smoke en QA
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141753F2-688C-483B-A0AE-80D4D22EF63E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CBDDBFF-D978-4538-875D-C8D07FD61674}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,19 +65,19 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>SMA017</t>
-  </si>
-  <si>
-    <t>ABC12SSMA017</t>
-  </si>
-  <si>
-    <t>ZAZ123SSMA017</t>
-  </si>
-  <si>
-    <t>SmokPreSiete</t>
-  </si>
-  <si>
-    <t>SmokePreProdNamSiete</t>
+    <t>SmokQADos</t>
+  </si>
+  <si>
+    <t>SmokeNameQADos</t>
+  </si>
+  <si>
+    <t>SMA018</t>
+  </si>
+  <si>
+    <t>ABC12SSMA018</t>
+  </si>
+  <si>
+    <t>ZAZ123SSMA018</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,16 +439,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>27100114</v>
+        <v>27100115</v>
       </c>
       <c r="D2">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -462,7 +462,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,7 +474,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
   </sheetData>
@@ -487,7 +487,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,13 +509,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -529,7 +529,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +541,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>21200117</v>
+        <v>21200118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se modifica Data para SmokeOcho en Preprod
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CBDDBFF-D978-4538-875D-C8D07FD61674}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A90CA82-8BF9-4A50-AB6B-FD2BCA0666DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,19 +65,19 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>SmokQADos</t>
-  </si>
-  <si>
-    <t>SmokeNameQADos</t>
-  </si>
-  <si>
-    <t>SMA018</t>
-  </si>
-  <si>
-    <t>ABC12SSMA018</t>
-  </si>
-  <si>
-    <t>ZAZ123SSMA018</t>
+    <t>SmokPreProdOcho</t>
+  </si>
+  <si>
+    <t>SmokeNamePreProdOcho</t>
+  </si>
+  <si>
+    <t>SMP019</t>
+  </si>
+  <si>
+    <t>ABC12SSMP019</t>
+  </si>
+  <si>
+    <t>ZAZ123SSMP019</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,10 +445,10 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <v>27100115</v>
+        <v>27100116</v>
       </c>
       <c r="D2">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -462,7 +462,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,7 +474,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
   </sheetData>
@@ -487,7 +487,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +541,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>21200118</v>
+        <v>21200119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se modifica data para hacer smoke en preProd
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A90CA82-8BF9-4A50-AB6B-FD2BCA0666DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756DB0C6-19B2-4013-B340-9B2DB099DC96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DatosCuenta" sheetId="1" r:id="rId1"/>
@@ -65,19 +65,19 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>SmokPreProdOcho</t>
-  </si>
-  <si>
-    <t>SmokeNamePreProdOcho</t>
-  </si>
-  <si>
-    <t>SMP019</t>
-  </si>
-  <si>
-    <t>ABC12SSMP019</t>
-  </si>
-  <si>
-    <t>ZAZ123SSMP019</t>
+    <t>SmokPreProdNueve</t>
+  </si>
+  <si>
+    <t>SmokeNamePreProdNueve</t>
+  </si>
+  <si>
+    <t>SMP020</t>
+  </si>
+  <si>
+    <t>ABC12SSMP020</t>
+  </si>
+  <si>
+    <t>ZAZ123SSMP020</t>
   </si>
 </sst>
 </file>
@@ -412,7 +412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -445,10 +445,10 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <v>27100116</v>
+        <v>27100117</v>
       </c>
       <c r="D2">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -474,7 +474,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
   </sheetData>
@@ -487,7 +487,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2DEA8B-0CD5-444B-B1FB-D4111E0F6DDF}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +541,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>21200119</v>
+        <v>21200120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se modifica la data para hacer smoke diez en pre prod
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756DB0C6-19B2-4013-B340-9B2DB099DC96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC817AB-7B11-4106-BFFF-1F3597C630D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DatosCuenta" sheetId="1" r:id="rId1"/>
@@ -65,19 +65,19 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>SmokPreProdNueve</t>
-  </si>
-  <si>
-    <t>SmokeNamePreProdNueve</t>
-  </si>
-  <si>
-    <t>SMP020</t>
-  </si>
-  <si>
-    <t>ABC12SSMP020</t>
-  </si>
-  <si>
-    <t>ZAZ123SSMP020</t>
+    <t>SmokPreProdDiez</t>
+  </si>
+  <si>
+    <t>SmokeNamePreProdDiez</t>
+  </si>
+  <si>
+    <t>SMP021</t>
+  </si>
+  <si>
+    <t>ABC12SSMP021</t>
+  </si>
+  <si>
+    <t>ZAZ123SSMP021</t>
   </si>
 </sst>
 </file>
@@ -412,7 +412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -445,10 +445,10 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <v>27100117</v>
+        <v>27100118</v>
       </c>
       <c r="D2">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -474,7 +474,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>638</v>
+        <v>639</v>
       </c>
     </row>
   </sheetData>
@@ -528,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2DEA8B-0CD5-444B-B1FB-D4111E0F6DDF}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +541,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>21200120</v>
+        <v>21200121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se sube data para hacer Smoke en "NombreAmbiente" Release: Nro.XXX
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Desktop\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC817AB-7B11-4106-BFFF-1F3597C630D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57E0FE2-3AC3-45EC-AB0D-244978F0D20A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DatosCuenta" sheetId="1" r:id="rId1"/>
@@ -412,8 +412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,7 +448,7 @@
         <v>27100118</v>
       </c>
       <c r="D2">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -528,7 +528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2DEA8B-0CD5-444B-B1FB-D4111E0F6DDF}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Se modifica data para Smoke en "NombreAmbiente". Release: Nro.XXX
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Desktop\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57E0FE2-3AC3-45EC-AB0D-244978F0D20A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E434B3-E88F-4DF4-9351-FFF3A32B2270}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -413,7 +413,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,7 +448,7 @@
         <v>27100118</v>
       </c>
       <c r="D2">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se modifica data para hacer prueba en QA
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC817AB-7B11-4106-BFFF-1F3597C630D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84A65D7-C83A-404C-83A8-D98F563F0B31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,12 +65,6 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>SmokPreProdDiez</t>
-  </si>
-  <si>
-    <t>SmokeNamePreProdDiez</t>
-  </si>
-  <si>
     <t>SMP021</t>
   </si>
   <si>
@@ -78,6 +72,12 @@
   </si>
   <si>
     <t>ZAZ123SSMP021</t>
+  </si>
+  <si>
+    <t>SmokQATres</t>
+  </si>
+  <si>
+    <t>SmokeNameQATres</t>
   </si>
 </sst>
 </file>
@@ -439,16 +439,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2">
-        <v>27100118</v>
+        <v>27100119</v>
       </c>
       <c r="D2">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -474,7 +474,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
   </sheetData>
@@ -509,13 +509,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -541,7 +541,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>21200121</v>
+        <v>21200122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se crearon recordings para verificar el directorio y si está o no el archivo polizas.csv y el recording para renombrar el archivo. Se modifica data la probar smoke en QA
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84A65D7-C83A-404C-83A8-D98F563F0B31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422FD3E4-21C3-46CC-90FE-9371C325A11D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DatosCuenta" sheetId="1" r:id="rId1"/>
@@ -65,19 +65,19 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>SMP021</t>
-  </si>
-  <si>
-    <t>ABC12SSMP021</t>
-  </si>
-  <si>
-    <t>ZAZ123SSMP021</t>
-  </si>
-  <si>
-    <t>SmokQATres</t>
-  </si>
-  <si>
-    <t>SmokeNameQATres</t>
+    <t>SmokQACuatro</t>
+  </si>
+  <si>
+    <t>SmokeNameQACUatro</t>
+  </si>
+  <si>
+    <t>SMP022</t>
+  </si>
+  <si>
+    <t>ABC12SSMP022</t>
+  </si>
+  <si>
+    <t>ZAZ123SSMP022</t>
   </si>
 </sst>
 </file>
@@ -412,7 +412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -439,16 +439,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>27100119</v>
+        <v>27100120</v>
       </c>
       <c r="D2">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -474,7 +474,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
   </sheetData>
@@ -509,13 +509,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -528,7 +528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2DEA8B-0CD5-444B-B1FB-D4111E0F6DDF}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -541,7 +541,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>21200122</v>
+        <v>21200123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se modifica data para Smoke en PreProd PC y BC
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422FD3E4-21C3-46CC-90FE-9371C325A11D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9ABCDA9-9C2D-4E51-B2E6-03637EF504B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DatosCuenta" sheetId="1" r:id="rId1"/>
@@ -65,19 +65,19 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>SmokQACuatro</t>
-  </si>
-  <si>
-    <t>SmokeNameQACUatro</t>
-  </si>
-  <si>
-    <t>SMP022</t>
-  </si>
-  <si>
-    <t>ABC12SSMP022</t>
-  </si>
-  <si>
-    <t>ZAZ123SSMP022</t>
+    <t>SMP023</t>
+  </si>
+  <si>
+    <t>ABC12SSMP023</t>
+  </si>
+  <si>
+    <t>ZAZ123SSMP023</t>
+  </si>
+  <si>
+    <t>SmokPreProdJune</t>
+  </si>
+  <si>
+    <t>SmokeNameJune</t>
   </si>
 </sst>
 </file>
@@ -412,7 +412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -439,13 +439,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2">
-        <v>27100120</v>
+        <v>27100121</v>
       </c>
       <c r="D2">
         <v>122</v>
@@ -509,13 +509,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -528,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2DEA8B-0CD5-444B-B1FB-D4111E0F6DDF}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
se sube para smoke en QA
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9ABCDA9-9C2D-4E51-B2E6-03637EF504B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A0584E-5F36-4542-8910-094B1AFA0866}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,19 +65,19 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>SMP023</t>
-  </si>
-  <si>
-    <t>ABC12SSMP023</t>
-  </si>
-  <si>
-    <t>ZAZ123SSMP023</t>
-  </si>
-  <si>
-    <t>SmokPreProdJune</t>
-  </si>
-  <si>
-    <t>SmokeNameJune</t>
+    <t>SmokPreProdJuneTres</t>
+  </si>
+  <si>
+    <t>SmokeNameJuneTres</t>
+  </si>
+  <si>
+    <t>SMP024</t>
+  </si>
+  <si>
+    <t>ABC12SSMP024</t>
+  </si>
+  <si>
+    <t>ZAZ123SSMP024</t>
   </si>
 </sst>
 </file>
@@ -439,16 +439,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>27100121</v>
+        <v>27100123</v>
       </c>
       <c r="D2">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -474,7 +474,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>641</v>
+        <v>643</v>
       </c>
     </row>
   </sheetData>
@@ -509,13 +509,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -529,7 +529,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +541,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>21200123</v>
+        <v>21200125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se modifica data para Smoke en PreProd R33
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke_new\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4904D3-A523-4DB1-9992-B2C99FDB8C7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE3ED97-2727-4F10-A701-77CF82ECE8BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,19 +65,19 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>SmokQAJuneCinco</t>
-  </si>
-  <si>
-    <t>SmokeNameQAJuneCinco</t>
-  </si>
-  <si>
-    <t>SMP029</t>
-  </si>
-  <si>
-    <t>ABC12SSMP029</t>
-  </si>
-  <si>
-    <t>ZAZ123SSMP029</t>
+    <t>SmokPreProdJuneOne</t>
+  </si>
+  <si>
+    <t>SmokeNamePreProdOne</t>
+  </si>
+  <si>
+    <t>SMP030</t>
+  </si>
+  <si>
+    <t>ABC12SSMP030</t>
+  </si>
+  <si>
+    <t>ZAZ123SSMP030</t>
   </si>
 </sst>
 </file>
@@ -445,10 +445,10 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <v>27100127</v>
+        <v>27100128</v>
       </c>
       <c r="D2">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -474,7 +474,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>647</v>
+        <v>648</v>
       </c>
     </row>
   </sheetData>
@@ -487,7 +487,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +541,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>21200128</v>
+        <v>21200129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se modifica data para Smoke en QA
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke_new\Smoke\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE00BEB7-B617-4371-911E-BF5C7E7267A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7469641A-46D6-4328-BC9F-525A31E8C194}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
@@ -65,12 +65,6 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>SmokPreProdJuneTwo</t>
-  </si>
-  <si>
-    <t>SmokeNamePreProTwo</t>
-  </si>
-  <si>
     <t>SMP031</t>
   </si>
   <si>
@@ -78,6 +72,12 @@
   </si>
   <si>
     <t>ZAZ123SSMP031</t>
+  </si>
+  <si>
+    <t>SmokQAJuneOne</t>
+  </si>
+  <si>
+    <t>SmokeNameQAJuneOne</t>
   </si>
 </sst>
 </file>
@@ -439,10 +439,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>27100128</v>
@@ -484,10 +484,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B4D3337-C598-431D-875D-6881D8F6F2F1}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+      <selection activeCell="A3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,24 +509,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se mejora las anulaciones y se modifica datos de sola la cuenta
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7469641A-46D6-4328-BC9F-525A31E8C194}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA88E9F9-B1A1-4BD2-B386-E992938B1E04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DatosCuenta" sheetId="1" r:id="rId1"/>
@@ -74,10 +74,10 @@
     <t>ZAZ123SSMP031</t>
   </si>
   <si>
-    <t>SmokQAJuneOne</t>
-  </si>
-  <si>
-    <t>SmokeNameQAJuneOne</t>
+    <t>SmokQAJuneTwo</t>
+  </si>
+  <si>
+    <t>SmokeNameQAJuneTwo</t>
   </si>
 </sst>
 </file>
@@ -412,8 +412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,10 +445,10 @@
         <v>13</v>
       </c>
       <c r="C2">
-        <v>27100128</v>
+        <v>27100129</v>
       </c>
       <c r="D2">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -528,7 +528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2DEA8B-0CD5-444B-B1FB-D4111E0F6DDF}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
se modifica data para SmokeQA 29-06-2021
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49FADAF7-632C-4B6C-8FD2-8DA48FCA64F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3C482A-74CE-48C7-A2A4-4E4B2ABC4E44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="3045" windowWidth="15375" windowHeight="7875" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DatosCuenta" sheetId="1" r:id="rId1"/>
@@ -65,19 +65,19 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>SmokQAPreProdJuneTwo</t>
-  </si>
-  <si>
-    <t>SmokeNamePreProdJuneTwo</t>
-  </si>
-  <si>
-    <t>SMP032</t>
-  </si>
-  <si>
-    <t>ABC12SSMP032</t>
-  </si>
-  <si>
-    <t>ZAZ123SSMP032</t>
+    <t>SmokQAJuneLast</t>
+  </si>
+  <si>
+    <t>SmokeNameQAJuneLast</t>
+  </si>
+  <si>
+    <t>SMP033</t>
+  </si>
+  <si>
+    <t>ABC12SSMP033</t>
+  </si>
+  <si>
+    <t>ZAZ123SSMP033</t>
   </si>
 </sst>
 </file>
@@ -445,10 +445,10 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <v>27100130</v>
+        <v>27100131</v>
       </c>
       <c r="D2">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -474,7 +474,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>650</v>
+        <v>651</v>
       </c>
     </row>
   </sheetData>
@@ -529,7 +529,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +541,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>21200131</v>
+        <v>21200132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se sube data para smoke QA 01-07-2021
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3C482A-74CE-48C7-A2A4-4E4B2ABC4E44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C908FD77-0574-4D39-8AB2-D1F25B9AFCC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,19 +65,19 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>SmokQAJuneLast</t>
-  </si>
-  <si>
-    <t>SmokeNameQAJuneLast</t>
-  </si>
-  <si>
-    <t>SMP033</t>
-  </si>
-  <si>
-    <t>ABC12SSMP033</t>
-  </si>
-  <si>
-    <t>ZAZ123SSMP033</t>
+    <t>SmokQAJuneLastOne</t>
+  </si>
+  <si>
+    <t>SmokeNameQAJuneLastOne</t>
+  </si>
+  <si>
+    <t>SMP034</t>
+  </si>
+  <si>
+    <t>ABC12SSMP034</t>
+  </si>
+  <si>
+    <t>ZAZ123SSMP034</t>
   </si>
 </sst>
 </file>
@@ -445,10 +445,10 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <v>27100131</v>
+        <v>27100132</v>
       </c>
       <c r="D2">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -474,7 +474,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>651</v>
+        <v>652</v>
       </c>
     </row>
   </sheetData>
@@ -529,7 +529,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +541,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>21200132</v>
+        <v>21200133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se modifica data para SmokeQA
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C908FD77-0574-4D39-8AB2-D1F25B9AFCC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A856B10F-685E-4C8F-ADC8-8A8E0B33479A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,19 +65,19 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>SmokQAJuneLastOne</t>
-  </si>
-  <si>
-    <t>SmokeNameQAJuneLastOne</t>
-  </si>
-  <si>
-    <t>SMP034</t>
-  </si>
-  <si>
-    <t>ABC12SSMP034</t>
-  </si>
-  <si>
-    <t>ZAZ123SSMP034</t>
+    <t>SmokQAJuneLastTwo</t>
+  </si>
+  <si>
+    <t>SmokeNameQAJuneLastTwo</t>
+  </si>
+  <si>
+    <t>SMP035</t>
+  </si>
+  <si>
+    <t>ABC12SSMP035</t>
+  </si>
+  <si>
+    <t>ZAZ123SSMP035</t>
   </si>
 </sst>
 </file>
@@ -445,10 +445,10 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <v>27100132</v>
+        <v>27100133</v>
       </c>
       <c r="D2">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -474,7 +474,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>652</v>
+        <v>653</v>
       </c>
     </row>
   </sheetData>
@@ -529,7 +529,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +541,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>21200133</v>
+        <v>21200134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se modifica data para SmokeQa 05-07-2021 R34
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A856B10F-685E-4C8F-ADC8-8A8E0B33479A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324D86F4-9EF4-4C83-9B22-078A712DA198}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,19 +65,19 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>SmokQAJuneLastTwo</t>
-  </si>
-  <si>
-    <t>SmokeNameQAJuneLastTwo</t>
-  </si>
-  <si>
-    <t>SMP035</t>
-  </si>
-  <si>
-    <t>ABC12SSMP035</t>
-  </si>
-  <si>
-    <t>ZAZ123SSMP035</t>
+    <t>SmokQAJuneLastThree</t>
+  </si>
+  <si>
+    <t>SmokeNameQAJuneLastThree</t>
+  </si>
+  <si>
+    <t>SMP036</t>
+  </si>
+  <si>
+    <t>ABC12SSMP036</t>
+  </si>
+  <si>
+    <t>ZAZ123SSMP036</t>
   </si>
 </sst>
 </file>
@@ -445,10 +445,10 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <v>27100133</v>
+        <v>27100134</v>
       </c>
       <c r="D2">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -474,7 +474,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>653</v>
+        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -529,7 +529,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +541,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>21200134</v>
+        <v>21200135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se modifica creacón de cuenta para que actualice si ya existe otra cuenta con ese DNI Se quitó print de pantalla en Emison Hogar porque le hacía click a cuenta e iba a Edición de cuenta.
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324D86F4-9EF4-4C83-9B22-078A712DA198}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D195C4A-2E59-41B7-B603-DCAC0F40289B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,19 +65,19 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>SmokQAJuneLastThree</t>
-  </si>
-  <si>
-    <t>SmokeNameQAJuneLastThree</t>
-  </si>
-  <si>
-    <t>SMP036</t>
-  </si>
-  <si>
-    <t>ABC12SSMP036</t>
-  </si>
-  <si>
-    <t>ZAZ123SSMP036</t>
+    <t>SMP038</t>
+  </si>
+  <si>
+    <t>ABC12SSMP038</t>
+  </si>
+  <si>
+    <t>ZAZ123SSMP038</t>
+  </si>
+  <si>
+    <t>SmokeName</t>
+  </si>
+  <si>
+    <t>Smoke</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,10 +439,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>27100134</v>
@@ -474,7 +474,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>654</v>
+        <v>655</v>
       </c>
     </row>
   </sheetData>
@@ -487,7 +487,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+      <selection activeCell="A3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,13 +509,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -529,7 +529,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +541,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>21200135</v>
+        <v>21200136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se modifica Data para Smoke en Qa 08-07-2021
</commit_message>
<xml_diff>
--- a/Smoke/MaestroData.xlsx
+++ b/Smoke/MaestroData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Desktop\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E434B3-E88F-4DF4-9351-FFF3A32B2270}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D7B529-186B-48C9-98E4-84B0EAA30EFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DatosCuenta" sheetId="1" r:id="rId1"/>
@@ -65,19 +65,19 @@
     <t>NumeroDocumento</t>
   </si>
   <si>
-    <t>SmokPreProdDiez</t>
-  </si>
-  <si>
-    <t>SmokeNamePreProdDiez</t>
-  </si>
-  <si>
-    <t>SMP021</t>
-  </si>
-  <si>
-    <t>ABC12SSMP021</t>
-  </si>
-  <si>
-    <t>ZAZ123SSMP021</t>
+    <t>SmokeName</t>
+  </si>
+  <si>
+    <t>SmokeLastName</t>
+  </si>
+  <si>
+    <t>SQA040</t>
+  </si>
+  <si>
+    <t>ABC12SSQA040</t>
+  </si>
+  <si>
+    <t>ZAZ123SSQA040</t>
   </si>
 </sst>
 </file>
@@ -412,8 +412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,10 +445,10 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <v>27100118</v>
+        <v>23100200</v>
       </c>
       <c r="D2">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -474,7 +474,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
   </sheetData>
@@ -487,7 +487,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2DEA8B-0CD5-444B-B1FB-D4111E0F6DDF}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +541,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>21200121</v>
+        <v>21200140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>